<commit_message>
refactor; fix svein harald
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/dms-addition-svein-harald.xlsx
+++ b/docs/artifacts/rules/dms-addition-svein-harald.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60659BF-EACB-49D5-ACBF-1FFA2F613AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D1DC56-EFCD-4764-80D9-0CF7EC94B944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="128">
   <si>
     <t>role</t>
   </si>
@@ -383,63 +383,12 @@
     <t>OnshoreSubstation</t>
   </si>
   <si>
+    <t>TransmissionSubstation</t>
+  </si>
+  <si>
     <t>Transmission</t>
   </si>
   <si>
-    <t>TransmissionSubstation</t>
-  </si>
-  <si>
-    <t>power:CircuitBreaker</t>
-  </si>
-  <si>
-    <t>power:CurrentTransformer</t>
-  </si>
-  <si>
-    <t>power:DisconnectSwitch</t>
-  </si>
-  <si>
-    <t>power:EnergyArea</t>
-  </si>
-  <si>
-    <t>power:EnergyConsumer</t>
-  </si>
-  <si>
-    <t>power:GeneratingUnit</t>
-  </si>
-  <si>
-    <t>power:GeoLocation</t>
-  </si>
-  <si>
-    <t>power:Meter</t>
-  </si>
-  <si>
-    <t>power:MultiLineString</t>
-  </si>
-  <si>
-    <t>power:Point</t>
-  </si>
-  <si>
-    <t>power:Polygon</t>
-  </si>
-  <si>
-    <t>power:PowerLine</t>
-  </si>
-  <si>
-    <t>power:Substation</t>
-  </si>
-  <si>
-    <t>power:VoltageLevel</t>
-  </si>
-  <si>
-    <t>power:VoltageTransformer</t>
-  </si>
-  <si>
-    <t>power:WindFarm</t>
-  </si>
-  <si>
-    <t>power:WindTurbine</t>
-  </si>
-  <si>
     <t>complete</t>
   </si>
   <si>
@@ -455,13 +404,13 @@
     <t>Energy Area 2</t>
   </si>
   <si>
-    <t>Generating Unit</t>
-  </si>
-  <si>
     <t>This is the second container for the Energy Area</t>
   </si>
   <si>
-    <t>This is the second container for the Generating Unit</t>
+    <t>Generating Unit 2</t>
+  </si>
+  <si>
+    <t>This is the second container for the GeneratingUnit</t>
   </si>
 </sst>
 </file>
@@ -860,13 +809,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="A1:B12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
     <col min="2" max="2" width="33.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -972,9 +919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,7 +1032,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>39</v>
@@ -1141,7 +1088,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>39</v>
@@ -1488,16 +1435,16 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
     <col min="2" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="31.44140625" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
@@ -1546,24 +1493,24 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1571,7 +1518,6 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1581,7 +1527,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:P1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3730,7 +3676,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:H1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3738,7 +3684,8 @@
     <col min="1" max="1" width="22.44140625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="31.44140625" customWidth="1"/>
-    <col min="4" max="7" width="13" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+    <col min="5" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3784,6 +3731,9 @@
       <c r="A3" t="s">
         <v>103</v>
       </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
       <c r="G3" t="b">
         <v>1</v>
       </c>
@@ -3828,6 +3778,9 @@
       <c r="A7" t="s">
         <v>78</v>
       </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
       <c r="G7" t="b">
         <v>1</v>
       </c>
@@ -3839,6 +3792,9 @@
       <c r="A8" t="s">
         <v>115</v>
       </c>
+      <c r="D8" t="s">
+        <v>88</v>
+      </c>
       <c r="G8" t="b">
         <v>1</v>
       </c>
@@ -3850,6 +3806,9 @@
       <c r="A9" t="s">
         <v>75</v>
       </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
       <c r="G9" t="b">
         <v>1</v>
       </c>
@@ -3883,6 +3842,9 @@
       <c r="A12" t="s">
         <v>105</v>
       </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
       <c r="G12" t="b">
         <v>1</v>
       </c>
@@ -3930,6 +3892,9 @@
       <c r="A16" t="s">
         <v>79</v>
       </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
       <c r="G16" t="b">
         <v>1</v>
       </c>
@@ -3941,6 +3906,9 @@
       <c r="A17" t="s">
         <v>107</v>
       </c>
+      <c r="D17" t="s">
+        <v>88</v>
+      </c>
       <c r="G17" t="b">
         <v>1</v>
       </c>
@@ -3952,6 +3920,9 @@
       <c r="A18" t="s">
         <v>117</v>
       </c>
+      <c r="D18" t="s">
+        <v>118</v>
+      </c>
       <c r="G18" t="b">
         <v>1</v>
       </c>
@@ -3963,6 +3934,9 @@
       <c r="A19" t="s">
         <v>68</v>
       </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
       <c r="G19" t="b">
         <v>1</v>
       </c>
@@ -3974,6 +3948,9 @@
       <c r="A20" t="s">
         <v>63</v>
       </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
       <c r="G20" t="b">
         <v>1</v>
       </c>
@@ -4005,24 +3982,30 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="D23" t="s">
+        <v>83</v>
       </c>
       <c r="G23" t="b">
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="D24" t="s">
+        <v>88</v>
       </c>
       <c r="G24" t="b">
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -4051,6 +4034,9 @@
       <c r="A27" t="s">
         <v>101</v>
       </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
       <c r="G27" t="b">
         <v>1</v>
       </c>
@@ -4061,6 +4047,9 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>109</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
       </c>
       <c r="G28" t="b">
         <v>1</v>
@@ -4091,8 +4080,9 @@
     <col min="1" max="1" width="24.44140625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="31.44140625" customWidth="1"/>
-    <col min="4" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
@@ -4127,141 +4117,156 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>121</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>124</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>125</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>126</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="F10" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>128</v>
+        <v>79</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
       <c r="F14" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="F15" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s">
-        <v>133</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>135</v>
+        <v>101</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>109</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -4305,7 +4310,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -4358,7 +4363,7 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
doc: upate svein harald
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/dms-addition-svein-harald.xlsx
+++ b/docs/artifacts/rules/dms-addition-svein-harald.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60080300-9B4C-4DCA-BB7B-68BFBA105878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89CE9F3-F045-4D9F-8E64-5667DD9A64A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="128">
   <si>
     <t>role</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>This is the second container for the GeneratingUnit</t>
+  </si>
+  <si>
+    <t>Immutable</t>
   </si>
 </sst>
 </file>
@@ -914,11 +917,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,15 +930,15 @@
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="25.44140625" customWidth="1"/>
-    <col min="7" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="25.44140625" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" customWidth="1"/>
-    <col min="13" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="25.44140625" customWidth="1"/>
-    <col min="16" max="16" width="17.44140625" customWidth="1"/>
+    <col min="7" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="25.44140625" customWidth="1"/>
+    <col min="17" max="17" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -954,8 +957,9 @@
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="Q1" s="7"/>
+    </row>
+    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -978,34 +982,37 @@
         <v>28</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>38</v>
       </c>
@@ -1026,24 +1033,27 @@
       <c r="H3" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="4"/>
+      <c r="P3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1060,8 +1070,9 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>42</v>
       </c>
@@ -1082,24 +1093,27 @@
       <c r="H5" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="5"/>
+      <c r="I5" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J5" s="5"/>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="5"/>
+      <c r="P5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="Q5" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1116,8 +1130,9 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -1136,24 +1151,27 @@
       <c r="H7" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J7" s="4"/>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="4"/>
+      <c r="L7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="M7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="4"/>
+      <c r="P7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>41</v>
       </c>
@@ -1172,24 +1190,27 @@
       <c r="H8" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="4"/>
+      <c r="L8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="M8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M8" s="4"/>
       <c r="N8" s="4"/>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="4"/>
+      <c r="P8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="Q8" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -1208,24 +1229,27 @@
       <c r="H9" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J9" s="4"/>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="4"/>
+      <c r="L9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="4"/>
+      <c r="P9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>41</v>
       </c>
@@ -1244,24 +1268,27 @@
       <c r="H10" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J10" s="4"/>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="4"/>
+      <c r="L10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="M10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="4"/>
+      <c r="P10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
@@ -1280,26 +1307,29 @@
       <c r="H11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="I11" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J11" s="4"/>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="4"/>
+      <c r="L11" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4" t="s">
+      <c r="N11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>41</v>
       </c>
@@ -1316,30 +1346,33 @@
         <v>1</v>
       </c>
       <c r="H12" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="J12" s="4"/>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="4"/>
+      <c r="L12" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4" t="s">
+      <c r="N12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="Q12" s="4" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1520,11 +1553,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:P66"/>
+  <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1533,15 +1566,15 @@
     <col min="2" max="2" width="20.44140625" customWidth="1"/>
     <col min="3" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="7" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" customWidth="1"/>
-    <col min="12" max="12" width="20.44140625" customWidth="1"/>
-    <col min="13" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="18.44140625" customWidth="1"/>
-    <col min="16" max="16" width="20.44140625" customWidth="1"/>
+    <col min="7" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" customWidth="1"/>
+    <col min="13" max="13" width="20.44140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="18.44140625" customWidth="1"/>
+    <col min="17" max="17" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -1560,8 +1593,9 @@
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="Q1" s="7"/>
+    </row>
+    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1584,34 +1618,37 @@
         <v>28</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
@@ -1630,24 +1667,27 @@
       <c r="H3" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="4"/>
+      <c r="P3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1664,8 +1704,9 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
@@ -1684,24 +1725,27 @@
       <c r="H5" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="5"/>
+      <c r="I5" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J5" s="5"/>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="5"/>
+      <c r="P5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="Q5" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1718,8 +1762,9 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>60</v>
       </c>
@@ -1738,24 +1783,27 @@
       <c r="H7" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J7" s="4"/>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="4"/>
+      <c r="L7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="M7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="4"/>
+      <c r="P7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1772,8 +1820,9 @@
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>38</v>
       </c>
@@ -1792,24 +1841,27 @@
       <c r="H9" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="5"/>
+      <c r="I9" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J9" s="5"/>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="5"/>
+      <c r="L9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="M9" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="M9" s="5"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="5" t="s">
+      <c r="O9" s="5"/>
+      <c r="P9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="Q9" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>38</v>
       </c>
@@ -1830,24 +1882,27 @@
       <c r="H10" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J10" s="5"/>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="5"/>
+      <c r="L10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="5" t="s">
+      <c r="O10" s="5"/>
+      <c r="P10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="Q10" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
@@ -1866,24 +1921,27 @@
       <c r="H11" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J11" s="5"/>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="5"/>
+      <c r="L11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="M11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="5"/>
       <c r="N11" s="5"/>
-      <c r="O11" s="5" t="s">
+      <c r="O11" s="5"/>
+      <c r="P11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="P11" s="5" t="s">
+      <c r="Q11" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -1902,24 +1960,27 @@
       <c r="H12" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="5"/>
+      <c r="I12" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J12" s="5"/>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="5"/>
+      <c r="L12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="M12" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="M12" s="5"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="5" t="s">
+      <c r="O12" s="5"/>
+      <c r="P12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="P12" s="5" t="s">
+      <c r="Q12" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1936,8 +1997,9 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>65</v>
       </c>
@@ -1956,24 +2018,27 @@
       <c r="H14" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J14" s="4"/>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="4"/>
+      <c r="L14" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="M14" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="4"/>
+      <c r="P14" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P14" s="4" t="s">
+      <c r="Q14" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>65</v>
       </c>
@@ -1994,24 +2059,27 @@
       <c r="H15" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="I15" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J15" s="4"/>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="4"/>
+      <c r="L15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="M15" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="4" t="s">
+      <c r="O15" s="4"/>
+      <c r="P15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>65</v>
       </c>
@@ -2030,24 +2098,27 @@
       <c r="H16" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="I16" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J16" s="4"/>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="M16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M16" s="4"/>
       <c r="N16" s="4"/>
-      <c r="O16" s="4" t="s">
+      <c r="O16" s="4"/>
+      <c r="P16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P16" s="4" t="s">
+      <c r="Q16" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2064,8 +2135,9 @@
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q17" s="4"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>42</v>
       </c>
@@ -2084,24 +2156,27 @@
       <c r="H18" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="5"/>
+      <c r="I18" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J18" s="5"/>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="5"/>
+      <c r="L18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="M18" s="5"/>
       <c r="N18" s="5"/>
-      <c r="O18" s="5" t="s">
+      <c r="O18" s="5"/>
+      <c r="P18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="P18" s="5" t="s">
+      <c r="Q18" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>42</v>
       </c>
@@ -2122,24 +2197,27 @@
       <c r="H19" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J19" s="5"/>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="5"/>
+      <c r="L19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="M19" s="5"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="5" t="s">
+      <c r="O19" s="5"/>
+      <c r="P19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="P19" s="5" t="s">
+      <c r="Q19" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>42</v>
       </c>
@@ -2158,24 +2236,27 @@
       <c r="H20" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="5"/>
+      <c r="I20" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J20" s="5"/>
-      <c r="K20" s="5" t="s">
+      <c r="K20" s="5"/>
+      <c r="L20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="M20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M20" s="5"/>
       <c r="N20" s="5"/>
-      <c r="O20" s="5" t="s">
+      <c r="O20" s="5"/>
+      <c r="P20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="P20" s="5" t="s">
+      <c r="Q20" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>42</v>
       </c>
@@ -2194,24 +2275,27 @@
       <c r="H21" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="5"/>
+      <c r="I21" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J21" s="5"/>
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="5"/>
+      <c r="L21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="M21" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="M21" s="5"/>
       <c r="N21" s="5"/>
-      <c r="O21" s="5" t="s">
+      <c r="O21" s="5"/>
+      <c r="P21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="P21" s="5" t="s">
+      <c r="Q21" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2228,8 +2312,9 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q22" s="5"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>70</v>
       </c>
@@ -2248,24 +2333,27 @@
       <c r="H23" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="4"/>
+      <c r="I23" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J23" s="4"/>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="4"/>
+      <c r="L23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="M23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M23" s="4"/>
       <c r="N23" s="4"/>
-      <c r="O23" s="4" t="s">
+      <c r="O23" s="4"/>
+      <c r="P23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="P23" s="4" t="s">
+      <c r="Q23" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2282,8 +2370,9 @@
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q24" s="4"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>71</v>
       </c>
@@ -2299,23 +2388,24 @@
         <v>74</v>
       </c>
       <c r="G25" s="5"/>
-      <c r="H25" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="5" t="s">
+      <c r="O25" s="5"/>
+      <c r="P25" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="P25" s="5" t="s">
+      <c r="Q25" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>71</v>
       </c>
@@ -2334,24 +2424,27 @@
       <c r="H26" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I26" s="5"/>
+      <c r="I26" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J26" s="5"/>
-      <c r="K26" s="5" t="s">
+      <c r="K26" s="5"/>
+      <c r="L26" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="5" t="s">
+      <c r="O26" s="5"/>
+      <c r="P26" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="P26" s="5" t="s">
+      <c r="Q26" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>71</v>
       </c>
@@ -2372,24 +2465,27 @@
       <c r="H27" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="5"/>
+      <c r="I27" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J27" s="5"/>
-      <c r="K27" s="5" t="s">
+      <c r="K27" s="5"/>
+      <c r="L27" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="5" t="s">
+      <c r="O27" s="5"/>
+      <c r="P27" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="P27" s="5" t="s">
+      <c r="Q27" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2406,8 +2502,9 @@
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q28" s="5"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>78</v>
       </c>
@@ -2423,23 +2520,24 @@
         <v>68</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="H29" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="4" t="s">
+      <c r="O29" s="4"/>
+      <c r="P29" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="P29" s="4" t="s">
+      <c r="Q29" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2456,8 +2554,9 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q30" s="4"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>68</v>
       </c>
@@ -2476,24 +2575,27 @@
       <c r="H31" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I31" s="5"/>
+      <c r="I31" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J31" s="5"/>
-      <c r="K31" s="5" t="s">
+      <c r="K31" s="5"/>
+      <c r="L31" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="L31" s="5" t="s">
+      <c r="M31" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="M31" s="5"/>
       <c r="N31" s="5"/>
-      <c r="O31" s="5" t="s">
+      <c r="O31" s="5"/>
+      <c r="P31" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="P31" s="5" t="s">
+      <c r="Q31" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>68</v>
       </c>
@@ -2512,24 +2614,27 @@
       <c r="H32" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I32" s="5"/>
+      <c r="I32" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J32" s="5"/>
-      <c r="K32" s="5" t="s">
+      <c r="K32" s="5"/>
+      <c r="L32" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="M32" s="5"/>
       <c r="N32" s="5"/>
-      <c r="O32" s="5" t="s">
+      <c r="O32" s="5"/>
+      <c r="P32" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="P32" s="5" t="s">
+      <c r="Q32" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2546,8 +2651,9 @@
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q33" s="5"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>63</v>
       </c>
@@ -2563,23 +2669,24 @@
         <v>68</v>
       </c>
       <c r="G34" s="4"/>
-      <c r="H34" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
-      <c r="O34" s="4" t="s">
+      <c r="O34" s="4"/>
+      <c r="P34" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="P34" s="4" t="s">
+      <c r="Q34" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2596,8 +2703,9 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q35" s="4"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>82</v>
       </c>
@@ -2616,24 +2724,27 @@
       <c r="H36" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I36" s="5"/>
+      <c r="I36" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J36" s="5"/>
-      <c r="K36" s="5" t="s">
+      <c r="K36" s="5"/>
+      <c r="L36" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="M36" s="5"/>
       <c r="N36" s="5"/>
-      <c r="O36" s="5" t="s">
+      <c r="O36" s="5"/>
+      <c r="P36" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="P36" s="5" t="s">
+      <c r="Q36" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>82</v>
       </c>
@@ -2654,24 +2765,27 @@
       <c r="H37" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I37" s="5"/>
+      <c r="I37" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J37" s="5"/>
-      <c r="K37" s="5" t="s">
+      <c r="K37" s="5"/>
+      <c r="L37" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="M37" s="5"/>
       <c r="N37" s="5"/>
-      <c r="O37" s="5" t="s">
+      <c r="O37" s="5"/>
+      <c r="P37" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="P37" s="5" t="s">
+      <c r="Q37" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>82</v>
       </c>
@@ -2690,24 +2804,27 @@
       <c r="H38" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="5"/>
+      <c r="I38" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J38" s="5"/>
-      <c r="K38" s="5" t="s">
+      <c r="K38" s="5"/>
+      <c r="L38" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="L38" s="5" t="s">
+      <c r="M38" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="M38" s="5"/>
       <c r="N38" s="5"/>
-      <c r="O38" s="5" t="s">
+      <c r="O38" s="5"/>
+      <c r="P38" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="P38" s="5" t="s">
+      <c r="Q38" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>82</v>
       </c>
@@ -2728,24 +2845,27 @@
       <c r="H39" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="5"/>
+      <c r="I39" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J39" s="5"/>
-      <c r="K39" s="5" t="s">
+      <c r="K39" s="5"/>
+      <c r="L39" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="M39" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="M39" s="5"/>
       <c r="N39" s="5"/>
-      <c r="O39" s="5" t="s">
+      <c r="O39" s="5"/>
+      <c r="P39" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="P39" s="5" t="s">
+      <c r="Q39" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2762,8 +2882,9 @@
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q40" s="5"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>87</v>
       </c>
@@ -2779,23 +2900,24 @@
         <v>56</v>
       </c>
       <c r="G41" s="4"/>
-      <c r="H41" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
-      <c r="O41" s="4" t="s">
+      <c r="O41" s="4"/>
+      <c r="P41" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P41" s="4" t="s">
+      <c r="Q41" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>87</v>
       </c>
@@ -2811,23 +2933,24 @@
         <v>59</v>
       </c>
       <c r="G42" s="4"/>
-      <c r="H42" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
-      <c r="O42" s="4" t="s">
+      <c r="O42" s="4"/>
+      <c r="P42" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P42" s="4" t="s">
+      <c r="Q42" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>87</v>
       </c>
@@ -2843,23 +2966,24 @@
         <v>60</v>
       </c>
       <c r="G43" s="4"/>
-      <c r="H43" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
-      <c r="O43" s="4" t="s">
+      <c r="O43" s="4"/>
+      <c r="P43" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P43" s="4" t="s">
+      <c r="Q43" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>87</v>
       </c>
@@ -2878,24 +3002,27 @@
       <c r="H44" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I44" s="4"/>
+      <c r="I44" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J44" s="4"/>
-      <c r="K44" s="4" t="s">
+      <c r="K44" s="4"/>
+      <c r="L44" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L44" s="4" t="s">
+      <c r="M44" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="M44" s="4"/>
       <c r="N44" s="4"/>
-      <c r="O44" s="4" t="s">
+      <c r="O44" s="4"/>
+      <c r="P44" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P44" s="4" t="s">
+      <c r="Q44" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>87</v>
       </c>
@@ -2916,24 +3043,27 @@
       <c r="H45" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I45" s="4"/>
+      <c r="I45" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J45" s="4"/>
-      <c r="K45" s="4" t="s">
+      <c r="K45" s="4"/>
+      <c r="L45" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L45" s="4" t="s">
+      <c r="M45" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="M45" s="4"/>
       <c r="N45" s="4"/>
-      <c r="O45" s="4" t="s">
+      <c r="O45" s="4"/>
+      <c r="P45" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P45" s="4" t="s">
+      <c r="Q45" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>87</v>
       </c>
@@ -2952,24 +3082,27 @@
       <c r="H46" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I46" s="4"/>
+      <c r="I46" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J46" s="4"/>
-      <c r="K46" s="4" t="s">
+      <c r="K46" s="4"/>
+      <c r="L46" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L46" s="4" t="s">
+      <c r="M46" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M46" s="4"/>
       <c r="N46" s="4"/>
-      <c r="O46" s="4" t="s">
+      <c r="O46" s="4"/>
+      <c r="P46" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P46" s="4" t="s">
+      <c r="Q46" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>87</v>
       </c>
@@ -2990,24 +3123,27 @@
       <c r="H47" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I47" s="4"/>
+      <c r="I47" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J47" s="4"/>
-      <c r="K47" s="4" t="s">
+      <c r="K47" s="4"/>
+      <c r="L47" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L47" s="4" t="s">
+      <c r="M47" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="M47" s="4"/>
       <c r="N47" s="4"/>
-      <c r="O47" s="4" t="s">
+      <c r="O47" s="4"/>
+      <c r="P47" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P47" s="4" t="s">
+      <c r="Q47" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>87</v>
       </c>
@@ -3026,24 +3162,27 @@
       <c r="H48" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I48" s="4"/>
+      <c r="I48" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J48" s="4"/>
-      <c r="K48" s="4" t="s">
+      <c r="K48" s="4"/>
+      <c r="L48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L48" s="4" t="s">
+      <c r="M48" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="4" t="s">
+      <c r="O48" s="4"/>
+      <c r="P48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P48" s="4" t="s">
+      <c r="Q48" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>87</v>
       </c>
@@ -3064,24 +3203,27 @@
       <c r="H49" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I49" s="4"/>
+      <c r="I49" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J49" s="4"/>
-      <c r="K49" s="4" t="s">
+      <c r="K49" s="4"/>
+      <c r="L49" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L49" s="4" t="s">
+      <c r="M49" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="4" t="s">
+      <c r="O49" s="4"/>
+      <c r="P49" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P49" s="4" t="s">
+      <c r="Q49" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>87</v>
       </c>
@@ -3100,24 +3242,27 @@
       <c r="H50" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I50" s="4"/>
+      <c r="I50" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J50" s="4"/>
-      <c r="K50" s="4" t="s">
+      <c r="K50" s="4"/>
+      <c r="L50" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L50" s="4" t="s">
+      <c r="M50" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="4" t="s">
+      <c r="O50" s="4"/>
+      <c r="P50" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P50" s="4" t="s">
+      <c r="Q50" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -3134,8 +3279,9 @@
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q51" s="4"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>86</v>
       </c>
@@ -3154,24 +3300,27 @@
       <c r="H52" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I52" s="5"/>
+      <c r="I52" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J52" s="5"/>
-      <c r="K52" s="5" t="s">
+      <c r="K52" s="5"/>
+      <c r="L52" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="L52" s="5" t="s">
+      <c r="M52" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="M52" s="5"/>
       <c r="N52" s="5"/>
-      <c r="O52" s="5" t="s">
+      <c r="O52" s="5"/>
+      <c r="P52" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="P52" s="5" t="s">
+      <c r="Q52" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -3188,8 +3337,9 @@
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
       <c r="P53" s="5"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q53" s="5"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>92</v>
       </c>
@@ -3210,24 +3360,27 @@
       <c r="H54" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I54" s="4"/>
+      <c r="I54" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J54" s="4"/>
-      <c r="K54" s="4" t="s">
+      <c r="K54" s="4"/>
+      <c r="L54" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="L54" s="4" t="s">
+      <c r="M54" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="4" t="s">
+      <c r="O54" s="4"/>
+      <c r="P54" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="P54" s="4" t="s">
+      <c r="Q54" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>92</v>
       </c>
@@ -3248,24 +3401,27 @@
       <c r="H55" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I55" s="4"/>
+      <c r="I55" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J55" s="4"/>
-      <c r="K55" s="4" t="s">
+      <c r="K55" s="4"/>
+      <c r="L55" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="L55" s="4" t="s">
+      <c r="M55" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="4" t="s">
+      <c r="O55" s="4"/>
+      <c r="P55" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="P55" s="4" t="s">
+      <c r="Q55" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -3282,8 +3438,9 @@
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
       <c r="P56" s="4"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q56" s="4"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>100</v>
       </c>
@@ -3299,23 +3456,24 @@
         <v>102</v>
       </c>
       <c r="G57" s="5"/>
-      <c r="H57" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
       <c r="M57" s="5"/>
       <c r="N57" s="5"/>
-      <c r="O57" s="5" t="s">
+      <c r="O57" s="5"/>
+      <c r="P57" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="P57" s="5" t="s">
+      <c r="Q57" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>100</v>
       </c>
@@ -3336,24 +3494,27 @@
       <c r="H58" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I58" s="5"/>
+      <c r="I58" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J58" s="5"/>
-      <c r="K58" s="5" t="s">
+      <c r="K58" s="5"/>
+      <c r="L58" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="L58" s="5" t="s">
+      <c r="M58" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="M58" s="5"/>
       <c r="N58" s="5"/>
-      <c r="O58" s="5" t="s">
+      <c r="O58" s="5"/>
+      <c r="P58" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="P58" s="5" t="s">
+      <c r="Q58" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>100</v>
       </c>
@@ -3374,24 +3535,27 @@
       <c r="H59" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="I59" s="5"/>
+      <c r="I59" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J59" s="5"/>
-      <c r="K59" s="5" t="s">
+      <c r="K59" s="5"/>
+      <c r="L59" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="L59" s="5" t="s">
+      <c r="M59" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="M59" s="5"/>
       <c r="N59" s="5"/>
-      <c r="O59" s="5" t="s">
+      <c r="O59" s="5"/>
+      <c r="P59" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="P59" s="5" t="s">
+      <c r="Q59" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>100</v>
       </c>
@@ -3407,23 +3571,24 @@
         <v>108</v>
       </c>
       <c r="G60" s="5"/>
-      <c r="H60" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
       <c r="M60" s="5"/>
       <c r="N60" s="5"/>
-      <c r="O60" s="5" t="s">
+      <c r="O60" s="5"/>
+      <c r="P60" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="P60" s="5" t="s">
+      <c r="Q60" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -3440,8 +3605,9 @@
       <c r="N61" s="5"/>
       <c r="O61" s="5"/>
       <c r="P61" s="5"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q61" s="5"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>108</v>
       </c>
@@ -3462,24 +3628,27 @@
       <c r="H62" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I62" s="4"/>
+      <c r="I62" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J62" s="4"/>
-      <c r="K62" s="4" t="s">
+      <c r="K62" s="4"/>
+      <c r="L62" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="L62" s="4" t="s">
+      <c r="M62" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="M62" s="4"/>
       <c r="N62" s="4"/>
-      <c r="O62" s="4" t="s">
+      <c r="O62" s="4"/>
+      <c r="P62" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="P62" s="4" t="s">
+      <c r="Q62" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>108</v>
       </c>
@@ -3498,24 +3667,27 @@
       <c r="H63" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I63" s="4"/>
+      <c r="I63" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J63" s="4"/>
-      <c r="K63" s="4" t="s">
+      <c r="K63" s="4"/>
+      <c r="L63" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="L63" s="4" t="s">
+      <c r="M63" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="M63" s="4"/>
       <c r="N63" s="4"/>
-      <c r="O63" s="4" t="s">
+      <c r="O63" s="4"/>
+      <c r="P63" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="P63" s="4" t="s">
+      <c r="Q63" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>108</v>
       </c>
@@ -3534,24 +3706,27 @@
       <c r="H64" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I64" s="4"/>
+      <c r="I64" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J64" s="4"/>
-      <c r="K64" s="4" t="s">
+      <c r="K64" s="4"/>
+      <c r="L64" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="L64" s="4" t="s">
+      <c r="M64" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="M64" s="4"/>
       <c r="N64" s="4"/>
-      <c r="O64" s="4" t="s">
+      <c r="O64" s="4"/>
+      <c r="P64" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="P64" s="4" t="s">
+      <c r="Q64" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>108</v>
       </c>
@@ -3570,24 +3745,27 @@
       <c r="H65" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I65" s="4"/>
+      <c r="I65" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J65" s="4"/>
-      <c r="K65" s="4" t="s">
+      <c r="K65" s="4"/>
+      <c r="L65" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="L65" s="4" t="s">
+      <c r="M65" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="M65" s="4"/>
       <c r="N65" s="4"/>
-      <c r="O65" s="4" t="s">
+      <c r="O65" s="4"/>
+      <c r="P65" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="P65" s="4" t="s">
+      <c r="Q65" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>108</v>
       </c>
@@ -3606,26 +3784,29 @@
       <c r="H66" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I66" s="4"/>
+      <c r="I66" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J66" s="4"/>
-      <c r="K66" s="4" t="s">
+      <c r="K66" s="4"/>
+      <c r="L66" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="L66" s="4" t="s">
+      <c r="M66" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="M66" s="4"/>
       <c r="N66" s="4"/>
-      <c r="O66" s="4" t="s">
+      <c r="O66" s="4"/>
+      <c r="P66" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="P66" s="4" t="s">
+      <c r="Q66" s="4" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>